<commit_message>
adicionado ataque com clicke e icone do launcher
</commit_message>
<xml_diff>
--- a/NinjaTheHappyHour/Documentos/Cópia de requisitosNinjaDefinitivo2 (1).xlsx
+++ b/NinjaTheHappyHour/Documentos/Cópia de requisitosNinjaDefinitivo2 (1).xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="280">
   <si>
     <t>O sistema deve ao iniciar a sua execução carregar a cena de logomarcas</t>
   </si>
@@ -551,7 +551,339 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">O sistema deve Executar uma neblasca em cenarios frios, a neblasca deve aplicar uma força equivalente a sua direção no personagem do jogador </t>
+      <t xml:space="preserve">O sistema deve escolher uma ação aleatoria para a neblasca a cada </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>10 segundos</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, dentre essas escolhas é possivel ventos para a esquerda, ou para a direita</t>
+    </r>
+  </si>
+  <si>
+    <t>O sistema deve escolher para o vento da neblasca uma direção (esquerda ou direita) ou Desligar o vento da neblasca a cada 20 segundos de forma randomica</t>
+  </si>
+  <si>
+    <t>O sistema deve sempre orientar os pés do personagem do jogador na mesma direção a da gravidade</t>
+  </si>
+  <si>
+    <t>O sistema deve causar dano de meio coração se o jogador colidir com qualquer inimigo</t>
+  </si>
+  <si>
+    <t>O sistema deve executar uma janela de Desempenho caso o jogador chegue ao final da faze</t>
+  </si>
+  <si>
+    <t>O sistema deve tocar a música tema em loop ao iniciar o menu. ( segundo GDD )</t>
+  </si>
+  <si>
+    <t>O sistema deve tocar um "som de pop"quando o mouse passar em cima de "novo jogo".</t>
+  </si>
+  <si>
+    <t>O sistema deve tocar um "som de pop" quando o mouse passar em cima de "opções".</t>
+  </si>
+  <si>
+    <t>O sistema deve tocar um "som de trun" quando o mouse passar em cima de "barra deslizante de som".</t>
+  </si>
+  <si>
+    <t>O sistema deve tocar um "som de trun" quando o mouse passar em cima de "barra deslizante de brilho".</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> O sistema deve tocar um "som de pop" quando o mouse passar em cima de "carregar jogo".</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> O sistema deve tocar um "som de pop" quando o mouse passar em cima de "sair do jogo". </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> O sistema deve tocar sons de espada quando o ícone do ninja passar sobre o ícone da fase e no nome do jogo jogador.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> O sistema deve tocar a música da fase em loop.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> O sistema deve tocar o som de "pulo" quando o jogador apertar a seta para cima. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> O sistema deve tocar o som de "aterrissar" quando o personagem aterissar no solo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> O sistema deve tocar o som de "passo" toda vez que o personagem andar. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> O sistema deve tocar o som de "tiro" quando os inimigos atirarem. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> O sistema deve tocar o som de "pulo" quando o personagem pousar e pular por cima da cabeça de um inimigo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> O sistema não deve tocar um som não característico da ação feita. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> O sistema deve tocar o som de "grama" quando o personagem andar sobre a grama. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> O sistema deve tocar o som de "água" quando o personagem andar sobre a água. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> O sistema deve tocar um som de "dano" quando o inimigo for atingido pela espada. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> O sistema deve tocar um som de "grito de agonia leve" quando o inimigo morrer. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> O sistema deve tocar um som de "moeda" quando o personagem ganhar sua recompensa. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> O sistema deve tocar um som de "granada" quando o inimigo atirar granada. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> O sistema deve tocar um som de "dano ninja" quando o personagem for atingido pelo inimig. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> O sistema deve tocar um som de "marcha funebre" quando o personagem morrer. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> O sistema deve tocar um som de "tambor" quando o mouse passar em cima de "reiniciar". </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> O sistema deve apresentar uma música triste no menu de game over, representando a derrota. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> O sistema deve tocar um som de "grito ninja" quando o mouse passar em cima de "sair do jogo".</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> O sistema deve tocar um som de "tambor alegre" quando o progresso for salvo. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> O sistema deve tocar a música do menu de pausa em loop, até que o jogador retorne ao jogo. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> O sistema deve tocar um som de "tambor" quando o mouse passar em cima de "continuar". </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> O sistema deve tocar a música da vitória quando o jogador terminar a fase. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> O sistema deve tocar um som de "Uhul" quando uma conquista for alcançada. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> O sistema deve tocar um som de "intro" quando o jogo sair do menu de pausa. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> O sistema deve tocar um som em loop para representar o barulho dos inimigos. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> O sistema deve tocar uma música em loop enquanto é apresentado os créditos. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> O sistema deve apresentar um som de "espada" se o jogador tocar em qualquer lugar da tela enquanto os créditos passam. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> O sistema deve tocar uma música em loop quando o boss da fase aparecer. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> O sistema não deve desligar os sons de combate, apenas a música da fase. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> O sistema deve apresentar sons fluidos e na hora certa. </t>
+  </si>
+  <si>
+    <t>O sistema deve tocar uma musica alegre enquanto o usuario estiver na loja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O sistema deve tocar um som de "negação" sempre que uma mensagem de erro aparecer </t>
+  </si>
+  <si>
+    <t xml:space="preserve">O sistema deve tocar im som de "caixa registradora" quando ele pagar algo na loja </t>
+  </si>
+  <si>
+    <t>O sistema deve tocar uma musicas variadas durante o menu de celeção de fases</t>
+  </si>
+  <si>
+    <t>O sistema deve tocar musicas tema das respectivas áreas do menu de seleção de fase</t>
+  </si>
+  <si>
+    <t>O sistema deve tocar "grito ninja" sempre que for introdizir uma fase</t>
+  </si>
+  <si>
+    <t>O sistema deve tocar "gemido" quando o inimigo de espada for bater</t>
+  </si>
+  <si>
+    <t>O sistema deve tocar "passos inimigos" sempre que os inimigos se movimentarem</t>
+  </si>
+  <si>
+    <t>O sistema deve tocar "agua" sempre que o inimigo andar sobre a agua</t>
+  </si>
+  <si>
+    <t>O sistema deve tocar "grama" sempre que um inimigo andar pela grama</t>
+  </si>
+  <si>
+    <t>O sitema deve tocar musica tema da fase com efeito de éco sempre que o personagem entrar em uma caverna</t>
+  </si>
+  <si>
+    <t>O sitema deve tocar musica tema da fase com efeito de abafado sempre que entrar na agua</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O sitema deve tocar som "blin" sempre que a estrela ninja acertar a parede </t>
+  </si>
+  <si>
+    <t>O sistema deve tocar som "tiro parede" quando o tiro do enimigos acertarem a parede</t>
+  </si>
+  <si>
+    <t>O sistema deve se o jogador perder todas as vidas (corações) remover uma chance e volta para o ultimo checkpoint</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">O sistema deve deslizar o personagem caso ele entre em contato com parede horizontal  o descendo de acordo com a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>metade da força gravidade conforme GDD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="3" tint="0.39997558519241921"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">O sistema deve conter </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>4 modelos de inimigos segundo GDD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Um de ataque curto, outro de ataque a longa distacia, um hibrido, e um de ataque aereo.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">O sistema deve aumentar em </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>50 pontos a pontuação do jogador segundo GDD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="3"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, quando ele matar um inimigo</t>
+    </r>
+  </si>
+  <si>
+    <t>O sistema deve definir o dano do inimigo voador a meio coração, e seu ataque será por um voo rasante, a cada 10 segundos</t>
+  </si>
+  <si>
+    <t>O sistema deve executar morte sem animação caso o personagem do jogador caia em um buraco reduzindo uma chance do jogador e voltando para o ultimo checkpoint</t>
+  </si>
+  <si>
+    <t>O sistema deve enviar os dados de progresso do jogador somente se o jogador estiver conectado com a internet</t>
+  </si>
+  <si>
+    <t>O sistema deve registrar o tempo que o jogador levou para jogar a faze, o nome da faze, a quantidade de inimigos mortos, e sua pontuação como progresso e suas moedas e enviar para o servidor externo no final da faze</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O sistema deve executar animação que indique ao jogador que a plataforma esta danificada e vai cair </t>
+  </si>
+  <si>
+    <t>O sistema deve eliminar o jogador caso ele seja esmagado por uma plataforma animada mas não executar a animação de morte apenas reduzir uma chance do jogador</t>
+  </si>
+  <si>
+    <t>O sistema deve adicionar o valor da moeda no contador de  moedas caso o jogador colida com a moeda</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">O sistema deve definir o dano inimigo de ataque curto a meio coração e seu ataque será a cada </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2 segundos conforme GDD</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>O sistema deve executar dano da bomba usando um raio de</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 10 metros</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, então todos os inimigos que estão nesse espaço morrem, a bomba leva 5 segundos para explodir</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">O sistema deve executar a morte do personagem caso ele encoste nos espinhos verticas independente de sua velocidade voltando para o ultimo checkpoint </t>
     </r>
     <r>
       <rPr>
@@ -566,7 +898,307 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">O sistema deve escolher uma ação aleatoria para a neblasca a cada </t>
+      <t xml:space="preserve">O sistema deve aumentar o nivel do jogador a cada </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1000 pontos segundo GDD</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">O sistema deve definir o dano inimigo hibrido </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>a meio coração</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, e seu ataque ocorrerá a cada </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3 segundos</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, de forma aleatoria ele escolhe ou disparar ou atacar </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>conforme GDD</t>
+    </r>
+  </si>
+  <si>
+    <t>O sistema deve eliminar o tiro do jogador ou do inimigo caso este atinja uma plataforma</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">O sistema deve animar a moeda criando uma "rotação" em torno de si mesma </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>conforme os itens do GDD</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">O sistema deve adicionar </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">10 moedas </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">no contador de moedas se o jogador pegar um item "saquinho de moedas" </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>conforme documento de intens do GDD</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>O sistema deve permitir que o personagem empurre caixas no jogo quando o</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> jogador apertar o botão "x" conforme o documento de comandos do  GDD</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>O sistema deve ter plataformas que se deslocam automaticamente na vertical, horizontal e diagonal indo e voltando</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> conforme documento de mecanica do GDD</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>O sistema deve definir o dano inimigo de ataque longo a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 1 coração</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, e seu ataque ocorrerá a cada 5 segundos </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>conforme documento de Inimigos do GDD</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">O Sistema deve limitar a velocidade do personagem em </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">*4 por segundo  metros segundo documento do personagem principal no GDD </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="3"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">para que não seja adicionado força horizontal infinita </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">O sistema deve entregar ao jogador </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3 chances conforme as regras do GDD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> no inicio da faze</t>
+    </r>
+  </si>
+  <si>
+    <t>O sistema deve entregar ao jogador 3 chances para jogar a mesma faze, se o jogador morrer ele perde uma chance e volta para o ultimo checkpoint caso tenha</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">O sistema deve Reduzir a fricção do personagem do jogador com o solo </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>pela metade conforme GDD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, se ele estiver sobre um solo gelado</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">O sistema deve ter animação de neve em diagonal que enfatize a neblasca caso o personagem do jogador esteja em uma faze fria ou nevosa </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>conforme documento de level design do GDD</t>
+    </r>
+  </si>
+  <si>
+    <t>O sistema deve animar a neve de acordo com sua direção se a neblasca estiver apontando para a direita ou para a esquerda</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">O sistema deve intercalar a direção do vento da neblasca, não permitindo que depois dos </t>
     </r>
     <r>
       <rPr>
@@ -586,198 +1218,158 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>, dentre essas escolhas é possivel ventos para a esquerda, ou para a direita</t>
-    </r>
-  </si>
-  <si>
-    <t>O sistema deve escolher para o vento da neblasca uma direção (esquerda ou direita) ou Desligar o vento da neblasca a cada 20 segundos de forma randomica</t>
-  </si>
-  <si>
-    <t>O sistema deve sempre orientar os pés do personagem do jogador na mesma direção a da gravidade</t>
-  </si>
-  <si>
-    <t>O sistema deve causar dano de meio coração se o jogador colidir com qualquer inimigo</t>
-  </si>
-  <si>
-    <t>O sistema deve executar uma janela de Desempenho caso o jogador chegue ao final da faze</t>
-  </si>
-  <si>
-    <t>O sistema deve tocar a música tema em loop ao iniciar o menu. ( segundo GDD )</t>
-  </si>
-  <si>
-    <t>O sistema deve tocar um "som de pop"quando o mouse passar em cima de "novo jogo".</t>
-  </si>
-  <si>
-    <t>O sistema deve tocar um "som de pop" quando o mouse passar em cima de "opções".</t>
-  </si>
-  <si>
-    <t>O sistema deve tocar um "som de trun" quando o mouse passar em cima de "barra deslizante de som".</t>
-  </si>
-  <si>
-    <t>O sistema deve tocar um "som de trun" quando o mouse passar em cima de "barra deslizante de brilho".</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> O sistema deve tocar um "som de pop" quando o mouse passar em cima de "carregar jogo".</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> O sistema deve tocar um "som de pop" quando o mouse passar em cima de "sair do jogo". </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> O sistema deve tocar sons de espada quando o ícone do ninja passar sobre o ícone da fase e no nome do jogo jogador.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> O sistema deve tocar a música da fase em loop.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> O sistema deve tocar o som de "pulo" quando o jogador apertar a seta para cima. </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> O sistema deve tocar o som de "aterrissar" quando o personagem aterissar no solo.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> O sistema deve tocar o som de "passo" toda vez que o personagem andar. </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> O sistema deve tocar o som de "tiro" quando os inimigos atirarem. </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> O sistema deve tocar o som de "pulo" quando o personagem pousar e pular por cima da cabeça de um inimigo.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> O sistema não deve tocar um som não característico da ação feita. </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> O sistema deve tocar o som de "grama" quando o personagem andar sobre a grama. </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> O sistema deve tocar o som de "água" quando o personagem andar sobre a água. </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> O sistema deve tocar um som de "dano" quando o inimigo for atingido pela espada. </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> O sistema deve tocar um som de "grito de agonia leve" quando o inimigo morrer. </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> O sistema deve tocar um som de "moeda" quando o personagem ganhar sua recompensa. </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> O sistema deve tocar um som de "granada" quando o inimigo atirar granada. </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> O sistema deve tocar um som de "dano ninja" quando o personagem for atingido pelo inimig. </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> O sistema deve tocar um som de "marcha funebre" quando o personagem morrer. </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> O sistema deve tocar um som de "tambor" quando o mouse passar em cima de "reiniciar". </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> O sistema deve apresentar uma música triste no menu de game over, representando a derrota. </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> O sistema deve tocar um som de "grito ninja" quando o mouse passar em cima de "sair do jogo".</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> O sistema deve tocar um som de "tambor alegre" quando o progresso for salvo. </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> O sistema deve tocar a música do menu de pausa em loop, até que o jogador retorne ao jogo. </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> O sistema deve tocar um som de "tambor" quando o mouse passar em cima de "continuar". </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> O sistema deve tocar a música da vitória quando o jogador terminar a fase. </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> O sistema deve tocar um som de "Uhul" quando uma conquista for alcançada. </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> O sistema deve tocar um som de "intro" quando o jogo sair do menu de pausa. </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> O sistema deve tocar um som em loop para representar o barulho dos inimigos. </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> O sistema deve tocar uma música em loop enquanto é apresentado os créditos. </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> O sistema deve apresentar um som de "espada" se o jogador tocar em qualquer lugar da tela enquanto os créditos passam. </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> O sistema deve tocar uma música em loop quando o boss da fase aparecer. </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> O sistema não deve desligar os sons de combate, apenas a música da fase. </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> O sistema deve apresentar sons fluidos e na hora certa. </t>
-  </si>
-  <si>
-    <t>O sistema deve tocar uma musica alegre enquanto o usuario estiver na loja</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O sistema deve tocar um som de "negação" sempre que uma mensagem de erro aparecer </t>
-  </si>
-  <si>
-    <t xml:space="preserve">O sistema deve tocar im som de "caixa registradora" quando ele pagar algo na loja </t>
-  </si>
-  <si>
-    <t>O sistema deve tocar uma musicas variadas durante o menu de celeção de fases</t>
-  </si>
-  <si>
-    <t>O sistema deve tocar musicas tema das respectivas áreas do menu de seleção de fase</t>
-  </si>
-  <si>
-    <t>O sistema deve tocar "grito ninja" sempre que for introdizir uma fase</t>
-  </si>
-  <si>
-    <t>O sistema deve tocar "gemido" quando o inimigo de espada for bater</t>
-  </si>
-  <si>
-    <t>O sistema deve tocar "passos inimigos" sempre que os inimigos se movimentarem</t>
-  </si>
-  <si>
-    <t>O sistema deve tocar "agua" sempre que o inimigo andar sobre a agua</t>
-  </si>
-  <si>
-    <t>O sistema deve tocar "grama" sempre que um inimigo andar pela grama</t>
-  </si>
-  <si>
-    <t>O sitema deve tocar musica tema da fase com efeito de éco sempre que o personagem entrar em uma caverna</t>
-  </si>
-  <si>
-    <t>O sitema deve tocar musica tema da fase com efeito de abafado sempre que entrar na agua</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O sitema deve tocar som "blin" sempre que a estrela ninja acertar a parede </t>
-  </si>
-  <si>
-    <t>O sistema deve tocar som "tiro parede" quando o tiro do enimigos acertarem a parede</t>
-  </si>
-  <si>
-    <t>O sistema deve se o jogador perder todas as vidas (corações) remover uma chance e volta para o ultimo checkpoint</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">O sistema deve deslizar o personagem caso ele entre em contato com parede horizontal  o descendo de acordo com a </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="5"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>metade da força gravidade conforme GDD</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="3" tint="0.39997558519241921"/>
+      <t xml:space="preserve"> repita a direção do vento</t>
+    </r>
+  </si>
+  <si>
+    <t>O sistema deve exercer gravidade que aponte para o centro das plataformas circulares caso o jogador se aproxime delas</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">O sistema deve restaurar a gravidade normal que aponta para baixo caso o jogador pule fora da plataforma circular a uma distancia de </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>15 metros segundo documento de level design</t>
+    </r>
+  </si>
+  <si>
+    <t>O sistema deve associar as imagens de fundo do cenario ao movimento do personagem do jogador, porem a imagem de fundo é 20% mais lenta que o jogador</t>
+  </si>
+  <si>
+    <t>O sistema deve executar uma animação de morte caso o jogador perca toda sua vida.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">O sistema deve permitir que o inimigo de "ataque curto" faça uma patrulha no cenario,  e se o personagem ficar a uma distancia proxima </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>segundo documento de inimigos do GDD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ele persegue o jogador</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">O sistema deve permitir que o "inimigo aereo" fique parado e quando o jogador estiver a uma distancia </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>conforme GDD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ele persegue o jogador a uma velocidade de 70% do jogador</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">O sistema deve permitir que o "inimigo hibrido" ataque a longa distacia e a curta </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>segundo GDD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, e se mova lentamente com velocidade de </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*1/4 da velocidade do jogador</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">O sistema deve com o inimigo de "ataque curto" atacar o jogador quando ele chegar muito perto </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>segundo documento de inimigos do GDD</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">O sistema deve permitir que o inimigo de "ataque a longa distancia" mire no jogador, e atire se ele estiver a uma distancia menor ou igual a um valor </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>segundo documento de inimigos do GDD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -786,21 +1378,51 @@
     </r>
   </si>
   <si>
-    <t>O sistema deve bloquear o movimento horizontal dos botões "A" e "D" enquanto o personagem desliza pela parede</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">O sistema deve conter </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="5"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>4 modelos de inimigos segundo GDD</t>
+    <t>O sistema deve conter para o personagem principal animações para as seguintes ações do jogador: correr,  movimento de "dash", pular, deslizar na parede, empurrar objetos, ataque fraco, ataque forte, morrer, idle "esperando", lançar objetos como kunais bombas e shuriken,</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">O sistema deve para algumas plataformas segundo GDD permitir que elas caiam quando o jogador ficar mais de 1 segundo sobre elas, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>conforme regras e mecanica do GDD</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>O sistema deve permitir que o jogador acione uma alavanca quando apertar o botão Z para acionar uma plataforma ou abrir uma porta</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> conforme regras e mecanicas no GDD</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">O sistema deve caso uma pedra ou o jogador esteja sobre um botão ser apertado </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">conforme regras e mecanicas doGDD </t>
     </r>
     <r>
       <rPr>
@@ -810,83 +1432,79 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>: Um de ataque curto, outro de ataque a longa distacia, um hibrido, e um de ataque aereo.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">O sistema deve aumentar em </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="5"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>50 pontos a pontuação do jogador segundo GDD</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="3"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, quando ele matar um inimigo</t>
-    </r>
-  </si>
-  <si>
-    <t>O sistema deve definir o dano do inimigo voador a meio coração, e seu ataque será por um voo rasante, a cada 10 segundos</t>
-  </si>
-  <si>
-    <t>O sistema deve executar morte sem animação caso o personagem do jogador caia em um buraco reduzindo uma chance do jogador e voltando para o ultimo checkpoint</t>
-  </si>
-  <si>
-    <t>O sistema deve enviar os dados de progresso do jogador somente se o jogador estiver conectado com a internet</t>
-  </si>
-  <si>
-    <t>O sistema deve registrar o tempo que o jogador levou para jogar a faze, o nome da faze, a quantidade de inimigos mortos, e sua pontuação como progresso e suas moedas e enviar para o servidor externo no final da faze</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O sistema deve executar animação que indique ao jogador que a plataforma esta danificada e vai cair </t>
-  </si>
-  <si>
-    <t>O sistema deve eliminar o jogador caso ele seja esmagado por uma plataforma animada mas não executar a animação de morte apenas reduzir uma chance do jogador</t>
-  </si>
-  <si>
-    <t>O sistema deve adicionar o valor da moeda no contador de  moedas caso o jogador colida com a moeda</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">O sistema deve definir o dano inimigo de ataque curto a meio coração e seu ataque será a cada </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="5"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2 segundos conforme GDD</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>O sistema deve executar dano da bomba usando um raio de</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="5"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 10 metros</t>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>O sistema deve caso o jogador capture um item especial de imortalidade garantir ao jogador imortalidade por 20 segundos</t>
+  </si>
+  <si>
+    <t>O sistema deve caso o jogador capture um item "especial" de lucro com moedas com um valor de multiplicação aleatorio entre 1 e 10 garantir ao jogador ganhar esse valor multiplicado pela moeda que ele capturou o mesmo vale para os pontos</t>
+  </si>
+  <si>
+    <r>
+      <t>O sistema deve atribuir ao inimigo de 1 a 5  coraçoes de vida de acordo com sua resistencia</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> conforme GDD</t>
+    </r>
+  </si>
+  <si>
+    <t>O sistema deve conter moedas em 3d para que quando animar seja animada sua parte lateral</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">O sistema deve conter itens especiais que multipliquem os atributos do jogador (velocidade 1 a 5 vezes, dano 1 a 10 vezes) ou os valores das moedas, pontos, dano multiplicados de 1 a 10 vezes por um tempo limitado em 20 segundos </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>segundo documento de itens especiais GDD</t>
+    </r>
+  </si>
+  <si>
+    <t>O sistema deve avisar o jogador mostrando uma mensagem sobre a caixa caso o jogador encoste na caixa dizendo que ela pode ser empurrada caso o jogador aperte X</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">O sistema deve conter espinhos de parede e chão nas fazes </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>segundo documento de level design do GDD e mecanicas</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>O sistema deve executar morte do personagem por perfuração nos espinhos "horizontais" caso sua velocidade seja maior que</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 2m por segundo o documento de mecânicas no GDD</t>
     </r>
     <r>
       <rPr>
@@ -896,12 +1514,132 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>, então todos os inimigos que estão nesse espaço morrem, a bomba leva 5 segundos para explodir</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">O sistema deve executar a morte do personagem caso ele encoste nos espinhos verticas independente de sua velocidade voltando para o ultimo checkpoint </t>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>O sistema deve conter as seguintes animações para o inimigo: ficar esperando, atacar, correr,morrer, sumir</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O sistema deve ativar a plataforma "manual" para se mover quando o jogador apertar um botão ou acionar uma alavanca </t>
+  </si>
+  <si>
+    <r>
+      <t>O sistema deve ter portas que abram automaticamente quando o jogador passar por seu sensor que</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> tem um raio de 3 metros conforme documentos de mecanicas no GDD </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>O sistema deve ter portas que abram manualmente com o apertar de um botão ou por alavancas de acordo com os</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> documentos de mecanicas e level design no GDD</t>
+    </r>
+  </si>
+  <si>
+    <t>O sistema deve permitir que a caixa que o jogador empurrar caia na cabeça de um inimigo e o destrua, assim também a caixa é destruída</t>
+  </si>
+  <si>
+    <r>
+      <t>O sistema deve valorizar as moedas que o jogador coleta da seguinte forma: se for ouro</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, se for prata </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> se for bronze</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 2,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> se for de ouro com diamante </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>10 conforme itens do GDD</t>
+    </r>
+  </si>
+  <si>
+    <t>O sistema deve retirar uma quantidade de vida do inimigo segundo GDD de acordo com o dano do ataque do personagem do jogador subtraindo pela resistencia do inimigo</t>
+  </si>
+  <si>
+    <t>O sistema deve quando o personagem do jogador sair da zona de visão da camera no eixo vertical fazer com que a camera reajuste sua posição  nesse eixo de forma que o jogador fique no centro da tela</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">O sistema deve Executar uma neblasca em cenarios frios, a neblasca deve aplicar 1,5 vezes força equivalente a sua direção no personagem do jogador </t>
     </r>
     <r>
       <rPr>
@@ -916,32 +1654,17 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">O sistema deve aumentar o nivel do jogador a cada </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="5"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1000 pontos segundo GDD</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">O sistema deve definir o dano inimigo hibrido </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="5"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>a meio coração</t>
+      <t xml:space="preserve">O sistema deve entregar a variação de força do inimigo seguindo os seguintes paramentros </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>segundo GDD:</t>
     </r>
     <r>
       <rPr>
@@ -951,749 +1674,11 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">, e seu ataque ocorrerá a cada </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="5"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>3 segundos</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="4"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, de forma aleatoria ele escolhe ou disparar ou atacar </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="5"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>conforme GDD</t>
-    </r>
-  </si>
-  <si>
-    <t>O sistema deve eliminar o tiro do jogador ou do inimigo caso este atinja uma plataforma</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">O sistema deve animar a moeda criando uma "rotação" em torno de si mesma </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="5"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>conforme os itens do GDD</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">O sistema deve adicionar </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="5"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">10 moedas </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="4"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">no contador de moedas se o jogador pegar um item "saquinho de moedas" </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="5"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>conforme documento de intens do GDD</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>O sistema deve permitir que o personagem empurre caixas no jogo quando o</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="5"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> jogador apertar o botão "x" conforme o documento de comandos do  GDD</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>O sistema deve ter plataformas que se deslocam automaticamente na vertical, horizontal e diagonal indo e voltando</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="5"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> conforme documento de mecanica do GDD</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>O sistema deve definir o dano inimigo de ataque longo a</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="5"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 1 coração</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="4"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, e seu ataque ocorrerá a cada 5 segundos </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="5"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>conforme documento de Inimigos do GDD</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="4"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">O Sistema deve limitar a velocidade do personagem em </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="5"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">*4 por segundo  metros segundo documento do personagem principal no GDD </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="3"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">para que não seja adicionado força horizontal infinita </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">O sistema deve entregar ao jogador </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="5"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>3 chances conforme as regras do GDD</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="4"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> no inicio da faze</t>
-    </r>
-  </si>
-  <si>
-    <t>O sistema deve entregar ao jogador 3 chances para jogar a mesma faze, se o jogador morrer ele perde uma chance e volta para o ultimo checkpoint caso tenha</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">O sistema deve Reduzir a fricção do personagem do jogador com o solo </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="5"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>pela metade conforme GDD</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="4"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, se ele estiver sobre um solo gelado</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">O sistema deve ter animação de neve em diagonal que enfatize a neblasca caso o personagem do jogador esteja em uma faze fria ou nevosa </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="5"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>conforme documento de level design do GDD</t>
-    </r>
-  </si>
-  <si>
-    <t>O sistema deve animar a neve de acordo com sua direção se a neblasca estiver apontando para a direita ou para a esquerda</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">O sistema deve intercalar a direção do vento da neblasca, não permitindo que depois dos </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="5"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>10 segundos</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="4"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> repita a direção do vento</t>
-    </r>
-  </si>
-  <si>
-    <t>O sistema deve exercer gravidade que aponte para o centro das plataformas circulares caso o jogador se aproxime delas</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">O sistema deve restaurar a gravidade normal que aponta para baixo caso o jogador pule fora da plataforma circular a uma distancia de </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="5"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>15 metros segundo documento de level design</t>
-    </r>
-  </si>
-  <si>
-    <t>O sistema deve associar as imagens de fundo do cenario ao movimento do personagem do jogador, porem a imagem de fundo é 20% mais lenta que o jogador</t>
-  </si>
-  <si>
-    <t>O sistema deve executar uma animação de morte caso o jogador perca toda sua vida.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">O sistema deve entregar a variação de força do inimigo seguindo os seguintes paramentros </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="5"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>segundo GDD:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="4"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> dano, forma de ataque, resistencia a dano</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">O sistema deve permitir que o inimigo de "ataque curto" faça uma patrulha no cenario,  e se o personagem ficar a uma distancia proxima </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="5"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>segundo documento de inimigos do GDD</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="4"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> ele persegue o jogador</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">O sistema deve permitir que o "inimigo aereo" fique parado e quando o jogador estiver a uma distancia </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="5"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>conforme GDD</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="4"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> ele persegue o jogador a uma velocidade de 70% do jogador</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">O sistema deve permitir que o "inimigo hibrido" ataque a longa distacia e a curta </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="5"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>segundo GDD</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="4"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, e se mova lentamente com velocidade de </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="5"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>*1/4 da velocidade do jogador</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="4"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">O sistema deve com o inimigo de "ataque curto" atacar o jogador quando ele chegar muito perto </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="5"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>segundo documento de inimigos do GDD</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">O sistema deve permitir que o inimigo de "ataque a longa distancia" mire no jogador, e atire se ele estiver a uma distancia menor ou igual a um valor </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="5"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>segundo documento de inimigos do GDD</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="4"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
-    <t>O sistema deve conter para o personagem principal animações para as seguintes ações do jogador: correr,  movimento de "dash", pular, deslizar na parede, empurrar objetos, ataque fraco, ataque forte, morrer, idle "esperando", lançar objetos como kunais bombas e shuriken,</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">O sistema deve para algumas plataformas segundo GDD permitir que elas caiam quando o jogador ficar mais de 1 segundo sobre elas, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="5"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>conforme regras e mecanica do GDD</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>O sistema deve permitir que o jogador acione uma alavanca quando apertar o botão Z para acionar uma plataforma ou abrir uma porta</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="5"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> conforme regras e mecanicas no GDD</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">O sistema deve caso uma pedra ou o jogador esteja sobre um botão ser apertado </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="5"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">conforme regras e mecanicas doGDD </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="4"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
-    <t>O sistema deve caso o jogador capture um item especial de imortalidade garantir ao jogador imortalidade por 20 segundos</t>
-  </si>
-  <si>
-    <t>O sistema deve caso o jogador capture um item "especial" de lucro com moedas com um valor de multiplicação aleatorio entre 1 e 10 garantir ao jogador ganhar esse valor multiplicado pela moeda que ele capturou o mesmo vale para os pontos</t>
-  </si>
-  <si>
-    <r>
-      <t>O sistema deve atribuir ao inimigo de 1 a 5  coraçoes de vida de acordo com sua resistencia</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="5"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> conforme GDD</t>
-    </r>
-  </si>
-  <si>
-    <t>O sistema deve conter moedas em 3d para que quando animar seja animada sua parte lateral</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">O sistema deve conter itens especiais que multipliquem os atributos do jogador (velocidade 1 a 5 vezes, dano 1 a 10 vezes) ou os valores das moedas, pontos, dano multiplicados de 1 a 10 vezes por um tempo limitado em 20 segundos </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="5"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>segundo documento de itens especiais GDD</t>
-    </r>
-  </si>
-  <si>
-    <t>O sistema deve avisar o jogador mostrando uma mensagem sobre a caixa caso o jogador encoste na caixa dizendo que ela pode ser empurrada caso o jogador aperte X</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">O sistema deve aumentar em 1 o numero de corações de vida de acordo com o nivel do jogador </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="5"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>a cada 1000 pontos conforme GDD no documento de regras e mecanicas</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">O sistema deve conter espinhos de parede e chão nas fazes </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="5"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>segundo documento de level design do GDD e mecanicas</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>O sistema deve executar morte do personagem por perfuração nos espinhos "horizontais" caso sua velocidade seja maior que</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="5"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 2m por segundo o documento de mecânicas no GDD</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="4"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
-    <t>O sistema deve conter as seguintes animações para o inimigo: ficar esperando, atacar, correr,morrer, sumir</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O sistema deve ativar a plataforma "manual" para se mover quando o jogador apertar um botão ou acionar uma alavanca </t>
-  </si>
-  <si>
-    <r>
-      <t>O sistema deve ter portas que abram automaticamente quando o jogador passar por seu sensor que</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="5"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> tem um raio de 3 metros conforme documentos de mecanicas no GDD </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>O sistema deve ter portas que abram manualmente com o apertar de um botão ou por alavancas de acordo com os</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> documentos de mecanicas e level design no GDD</t>
-    </r>
-  </si>
-  <si>
-    <t>O sistema deve permitir que a caixa que o jogador empurrar caia na cabeça de um inimigo e o destrua, assim também a caixa é destruída</t>
-  </si>
-  <si>
-    <r>
-      <t>O sistema deve valorizar as moedas que o jogador coleta da seguinte forma: se for ouro</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="5"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 5</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="4"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, se for prata </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="5"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>3,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="4"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> se for bronze</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="5"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 2,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="4"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> se for de ouro com diamante </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="5"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>10 conforme itens do GDD</t>
-    </r>
-  </si>
-  <si>
-    <t>O sistema deve retirar uma quantidade de vida do inimigo segundo GDD de acordo com o dano do ataque do personagem do jogador subtraindo pela resistencia do inimigo</t>
-  </si>
-  <si>
-    <t>O sistema deve quando o personagem do jogador sair da zona de visão da camera no eixo vertical fazer com que a camera reajuste sua posição  nesse eixo de forma que o jogador fique no centro da tela</t>
+      <t xml:space="preserve"> dano, forma de ataque, resistencia </t>
+    </r>
+  </si>
+  <si>
+    <t>O sistema deve aumentar em 1 o numero de corações de vida de acordo com o nivel do jogador a cada 1000 pontos conforme GDD no documento de regras e mecanicas</t>
   </si>
 </sst>
 </file>
@@ -1875,7 +1860,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1961,6 +1946,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2264,10 +2255,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A292"/>
+  <dimension ref="A1:A291"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A222" workbookViewId="0">
-      <selection activeCell="A229" sqref="A229"/>
+    <sheetView tabSelected="1" topLeftCell="A143" workbookViewId="0">
+      <selection activeCell="A161" sqref="A161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3048,7 +3039,7 @@
     </row>
     <row r="155" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.25">
@@ -3068,12 +3059,12 @@
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A159" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A160" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.25">
@@ -3088,12 +3079,12 @@
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A163" s="5" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A164" s="26" t="s">
-        <v>221</v>
+      <c r="A164" s="33" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.25">
@@ -3113,312 +3104,312 @@
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A169" s="4" t="s">
-        <v>162</v>
+        <v>277</v>
       </c>
     </row>
     <row r="170" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A170" s="4" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A171" s="4" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A172" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A175" s="4" t="s">
-        <v>222</v>
+      <c r="A175" s="1" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
-        <v>165</v>
+        <v>248</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A178" s="11" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="178" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A178" s="1" t="s">
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A179" s="10" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A179" s="11" t="s">
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A180" s="4" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A181" s="30" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A182" s="29" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A183" s="4" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A180" s="10" t="s">
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A185" s="4" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A186" s="27" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A181" s="4" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A182" s="30" t="s">
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A187" s="4" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A183" s="29" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="184" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A184" s="4" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A185" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="186" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A186" s="4" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A187" s="27" t="s">
-        <v>256</v>
-      </c>
-    </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A188" s="4" t="s">
-        <v>257</v>
+      <c r="A188" s="7" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A189" s="7" t="s">
-        <v>224</v>
+      <c r="A189" s="4" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A190" s="4" t="s">
-        <v>232</v>
+        <v>240</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A191" s="4" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A192" s="4" t="s">
-        <v>236</v>
+        <v>223</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A193" s="4" t="s">
-        <v>225</v>
+        <v>165</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A194" s="4" t="s">
-        <v>166</v>
+        <v>233</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A195" s="4" t="s">
-        <v>235</v>
+      <c r="A195" s="34" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A196" s="4" t="s">
-        <v>270</v>
+      <c r="A196" s="8" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A197" s="8" t="s">
-        <v>271</v>
+      <c r="A197" s="4" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A198" s="4" t="s">
-        <v>226</v>
+        <v>268</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A199" s="4" t="s">
-        <v>272</v>
+        <v>232</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A200" s="4" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A201" s="4" t="s">
-        <v>273</v>
+        <v>257</v>
       </c>
     </row>
     <row r="202" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A202" s="4" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="203" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A203" s="4" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A204" s="4" t="s">
+      <c r="A204" s="11" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A205" s="12" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A206" s="4" t="s">
         <v>227</v>
-      </c>
-    </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A205" s="11" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A206" s="12" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A207" s="4" t="s">
-        <v>229</v>
+        <v>270</v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A208" s="4" t="s">
-        <v>274</v>
+      <c r="A208" s="9" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A209" s="9" t="s">
-        <v>262</v>
+      <c r="A209" s="4" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A210" s="4" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A211" s="4" t="s">
-        <v>276</v>
+      <c r="A211" s="3" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A212" s="3" t="s">
-        <v>230</v>
+      <c r="A212" s="10" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A213" s="10" t="s">
-        <v>263</v>
+      <c r="A213" s="3" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="214" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A214" s="3" t="s">
-        <v>240</v>
+      <c r="A214" s="4" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="215" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A215" s="4" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
     </row>
     <row r="216" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A216" s="4" t="s">
-        <v>277</v>
+        <v>231</v>
       </c>
     </row>
     <row r="217" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A217" s="4" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="218" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A218" s="4" t="s">
-        <v>231</v>
+        <v>274</v>
       </c>
     </row>
     <row r="219" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A219" s="4" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A220" s="4" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="221" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A221" s="4" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A222" s="3" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="223" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A223" s="4" t="s">
         <v>265</v>
       </c>
     </row>
+    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A221" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="222" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A222" s="4" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="223" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A223" s="3" t="s">
+        <v>263</v>
+      </c>
+    </row>
     <row r="224" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A224" s="3" t="s">
-        <v>266</v>
+      <c r="A224" s="4" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="225" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A225" s="4" t="s">
-        <v>279</v>
+        <v>236</v>
       </c>
     </row>
     <row r="226" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A226" s="4" t="s">
-        <v>238</v>
+      <c r="A226" s="3" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="227" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A227" s="3" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A228" s="31" t="s">
+      <c r="A227" s="31" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A228" s="32" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="229" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A229" s="13" t="s">
         <v>167</v>
-      </c>
-    </row>
-    <row r="229" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A229" s="32" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="230" spans="1:1" x14ac:dyDescent="0.25">
@@ -3677,9 +3668,7 @@
       </c>
     </row>
     <row r="281" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A281" s="13" t="s">
-        <v>219</v>
-      </c>
+      <c r="A281" s="28"/>
     </row>
     <row r="282" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A282" s="28"/>
@@ -3710,9 +3699,6 @@
     </row>
     <row r="291" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A291" s="28"/>
-    </row>
-    <row r="292" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A292" s="28"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>